<commit_message>
Headers and Templates back-end integrated
</commit_message>
<xml_diff>
--- a/scrubFolder/de_scrubbing_output.xlsx
+++ b/scrubFolder/de_scrubbing_output.xlsx
@@ -376,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AE5"/>
+  <dimension ref="A1:AE6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -480,65 +480,17 @@
       <c r="A2" t="str">
         <v>9123456789</v>
       </c>
-      <c r="J2" t="b">
-        <v>1</v>
-      </c>
       <c r="K2" t="b">
         <v>1</v>
       </c>
-      <c r="L2" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" t="b">
-        <v>1</v>
-      </c>
       <c r="N2" t="b">
         <v>1</v>
       </c>
-      <c r="O2" t="b">
-        <v>1</v>
-      </c>
-      <c r="P2" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="b">
-        <v>1</v>
-      </c>
-      <c r="R2" t="b">
-        <v>1</v>
-      </c>
-      <c r="S2" t="b">
-        <v>1</v>
-      </c>
       <c r="T2" t="b">
         <v>1</v>
       </c>
-      <c r="U2" t="b">
-        <v>1</v>
-      </c>
-      <c r="V2" t="b">
-        <v>1</v>
-      </c>
-      <c r="W2" t="b">
-        <v>1</v>
-      </c>
-      <c r="X2" t="b">
-        <v>1</v>
-      </c>
       <c r="Y2" t="b">
         <v>1</v>
-      </c>
-      <c r="Z2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC2" t="b">
-        <v>0</v>
       </c>
       <c r="AD2" t="b">
         <v>0</v>
@@ -551,65 +503,17 @@
       <c r="A3" t="str">
         <v>9123456794</v>
       </c>
-      <c r="J3" t="b">
-        <v>1</v>
-      </c>
       <c r="K3" t="b">
         <v>1</v>
       </c>
-      <c r="L3" t="b">
-        <v>1</v>
-      </c>
-      <c r="M3" t="b">
-        <v>1</v>
-      </c>
       <c r="N3" t="b">
         <v>1</v>
       </c>
-      <c r="O3" t="b">
-        <v>1</v>
-      </c>
-      <c r="P3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R3" t="b">
-        <v>1</v>
-      </c>
-      <c r="S3" t="b">
-        <v>1</v>
-      </c>
       <c r="T3" t="b">
         <v>0</v>
       </c>
-      <c r="U3" t="b">
-        <v>1</v>
-      </c>
-      <c r="V3" t="b">
-        <v>1</v>
-      </c>
-      <c r="W3" t="b">
-        <v>1</v>
-      </c>
-      <c r="X3" t="b">
-        <v>1</v>
-      </c>
       <c r="Y3" t="b">
         <v>0</v>
-      </c>
-      <c r="Z3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AB3" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC3" t="b">
-        <v>1</v>
       </c>
       <c r="AD3" t="b">
         <v>1</v>
@@ -622,65 +526,17 @@
       <c r="A4" t="str">
         <v>9123456799</v>
       </c>
-      <c r="J4" t="b">
-        <v>1</v>
-      </c>
       <c r="K4" t="b">
         <v>1</v>
       </c>
-      <c r="L4" t="b">
-        <v>1</v>
-      </c>
-      <c r="M4" t="b">
-        <v>1</v>
-      </c>
       <c r="N4" t="b">
         <v>1</v>
       </c>
-      <c r="O4" t="b">
-        <v>1</v>
-      </c>
-      <c r="P4" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="b">
-        <v>1</v>
-      </c>
-      <c r="R4" t="b">
-        <v>1</v>
-      </c>
-      <c r="S4" t="b">
-        <v>1</v>
-      </c>
       <c r="T4" t="b">
         <v>1</v>
       </c>
-      <c r="U4" t="b">
-        <v>1</v>
-      </c>
-      <c r="V4" t="b">
-        <v>1</v>
-      </c>
-      <c r="W4" t="b">
-        <v>1</v>
-      </c>
-      <c r="X4" t="b">
-        <v>1</v>
-      </c>
       <c r="Y4" t="b">
         <v>1</v>
-      </c>
-      <c r="Z4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA4" t="b">
-        <v>0</v>
-      </c>
-      <c r="AB4" t="b">
-        <v>1</v>
-      </c>
-      <c r="AC4" t="b">
-        <v>0</v>
       </c>
       <c r="AD4" t="b">
         <v>0</v>
@@ -693,76 +549,51 @@
       <c r="A5" t="str">
         <v>9123456804</v>
       </c>
-      <c r="J5" t="b">
-        <v>1</v>
-      </c>
       <c r="K5" t="b">
         <v>1</v>
       </c>
-      <c r="L5" t="b">
-        <v>1</v>
-      </c>
-      <c r="M5" t="b">
-        <v>0</v>
-      </c>
       <c r="N5" t="b">
         <v>1</v>
       </c>
-      <c r="O5" t="b">
-        <v>1</v>
-      </c>
-      <c r="P5" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="b">
-        <v>1</v>
-      </c>
-      <c r="R5" t="b">
-        <v>0</v>
-      </c>
-      <c r="S5" t="b">
-        <v>1</v>
-      </c>
       <c r="T5" t="b">
         <v>0</v>
       </c>
-      <c r="U5" t="b">
-        <v>1</v>
-      </c>
-      <c r="V5" t="b">
-        <v>1</v>
-      </c>
-      <c r="W5" t="b">
-        <v>1</v>
-      </c>
-      <c r="X5" t="b">
-        <v>1</v>
-      </c>
       <c r="Y5" t="b">
         <v>0</v>
       </c>
-      <c r="Z5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AA5" t="b">
-        <v>1</v>
-      </c>
-      <c r="AB5" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC5" t="b">
-        <v>1</v>
-      </c>
       <c r="AD5" t="b">
         <v>1</v>
       </c>
       <c r="AE5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>9123456809</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="N6" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Y6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AD6" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE6" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AE5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AE6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>